<commit_message>
day2 - added some code
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E94D68-D5C5-4589-BD61-740EF19745EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765130FF-1C95-4313-AED7-3DB3CB019FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Column Name" sheetId="1" r:id="rId1"/>
     <sheet name="Table Name" sheetId="2" r:id="rId2"/>
     <sheet name="Allow" sheetId="3" r:id="rId3"/>
-    <sheet name="Show filter" sheetId="6" r:id="rId4"/>
-    <sheet name="Ag grid" sheetId="7" r:id="rId5"/>
-    <sheet name="Scenario" sheetId="5" r:id="rId6"/>
-    <sheet name="General" sheetId="9" r:id="rId7"/>
-    <sheet name="Submodule" sheetId="10" r:id="rId8"/>
-    <sheet name="Functionality" sheetId="11" r:id="rId9"/>
+    <sheet name="output" sheetId="12" r:id="rId4"/>
+    <sheet name="Show filter" sheetId="6" r:id="rId5"/>
+    <sheet name="Ag grid" sheetId="7" r:id="rId6"/>
+    <sheet name="Scenario" sheetId="5" r:id="rId7"/>
+    <sheet name="General" sheetId="9" r:id="rId8"/>
+    <sheet name="Submodule" sheetId="10" r:id="rId9"/>
+    <sheet name="Functionality" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1440,6 +1441,326 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9CE13C-18B1-46E1-9D59-9762715224E3}">
+  <dimension ref="A1:A61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF46B54-6C97-4087-92B3-46A6F07FECD3}">
   <dimension ref="A1:K3"/>
@@ -1574,7 +1895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90C649A-68FE-4FD8-B774-55C43AC88693}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
@@ -1726,6 +2047,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50A4355-EB3D-4087-82FB-962962930A4A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860EEA4A-358A-42BD-BA39-AEB2FC7F7214}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1906,7 +2239,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B880F16-291A-4C1E-93BE-F9F1E6E07C97}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2009,7 +2342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B3C02E-1F22-4F05-8AB3-7C88B4798301}">
   <dimension ref="A1:A7"/>
   <sheetViews>
@@ -2062,7 +2395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B945DD-8A55-447B-9441-D98FD531C25E}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2167,7 +2500,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D0BC2D-8A55-4356-9494-08BF8E26DA29}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -2260,324 +2593,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9CE13C-18B1-46E1-9D59-9762715224E3}">
-  <dimension ref="A1:A61"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A61"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>183</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>